<commit_message>
SPIFFS file system for html, latching relay logic
</commit_message>
<xml_diff>
--- a/PCB/BOM/BOM_PartType-SmartSwitch.xlsx
+++ b/PCB/BOM/BOM_PartType-SmartSwitch.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonathan\Documents\GitHub\SmartSwitch\PCB\BOM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonathan\Documents\GitHub\SmartSwitch\pcb\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDA48C08-CAD1-4D8A-89FC-D64A05C71C49}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C45446FC-C9DC-4813-B2B8-E5C4FB182B33}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F5D0A2F6-1853-4C1A-BB2F-2967265568D0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CEE4390B-974B-40B4-A16B-2C2F562EAE7A}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM_PartType-SmartSwitch" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="59">
   <si>
     <t>Comment</t>
   </si>
@@ -63,21 +63,27 @@
     <t>10uF</t>
   </si>
   <si>
-    <t>Capacitor; Alum Electrolytic; Cap 10 uF; Tol 20%; Vol-Rtg 25 VDC; SMT; 4x5.8; Tape&amp;Reel</t>
-  </si>
-  <si>
-    <t>C1</t>
-  </si>
-  <si>
-    <t>EEEFK1E100AR</t>
+    <t>Cap, Alu Elec, 1uf, 50v, Rad</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>ESK105M050AC3AA</t>
   </si>
   <si>
     <t>RESET</t>
   </si>
   <si>
+    <t>LED Uni-Color Red 645nm 2-Pin T-1 3/4</t>
+  </si>
+  <si>
     <t>D1</t>
   </si>
   <si>
+    <t>HLMP-D150</t>
+  </si>
+  <si>
     <t>SET</t>
   </si>
   <si>
@@ -120,9 +126,6 @@
     <t>PS1</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>DMN65D87</t>
   </si>
   <si>
@@ -162,52 +165,49 @@
     <t>RL</t>
   </si>
   <si>
-    <t>EG1218</t>
-  </si>
-  <si>
-    <t>Slide Switch, 500 V, -20 to 70 degC, 3-Pin THD, RoHS</t>
-  </si>
-  <si>
-    <t>SW1</t>
+    <t>U1</t>
+  </si>
+  <si>
+    <t>1N4148</t>
+  </si>
+  <si>
+    <t>Diode: switching; SMD; 100V; 0.15A; 4ns; 400mW; Package: reel, tape</t>
   </si>
   <si>
     <t>VD1, VD2</t>
   </si>
   <si>
-    <t>External 5V</t>
-  </si>
-  <si>
-    <t>Wire-To-Board Terminal Block, 2, 150 V, 10 A, 30 Awg, 16 Awg, 1.4 Mm</t>
-  </si>
-  <si>
-    <t>VIN_EXT</t>
-  </si>
-  <si>
-    <t>DMN65D87-L</t>
-  </si>
-  <si>
-    <t>‎ERJ-3EKF3300V‎</t>
-  </si>
-  <si>
-    <t>282834-2</t>
-  </si>
-  <si>
-    <t>1N4148W-TP‎</t>
-  </si>
-  <si>
-    <t>DIODE GEN PURP 100V 150MA SOD123</t>
+    <t>1N4148W</t>
+  </si>
+  <si>
+    <t>TL750L05CKCS</t>
+  </si>
+  <si>
+    <t>IC REG LINEAR 5V 150MA TO220-3</t>
+  </si>
+  <si>
+    <t>ERJ-3EKF3300V</t>
+  </si>
+  <si>
+    <t>5111F5</t>
   </si>
   <si>
     <t>LED GREEN 5/32" HOLE PANEL MOUNT</t>
   </si>
   <si>
-    <t>5111F5</t>
-  </si>
-  <si>
     <t>5111F1</t>
   </si>
   <si>
     <t>LED RED 5/32" HOLE PANEL MOUNT</t>
+  </si>
+  <si>
+    <t>RRA1GC1100</t>
+  </si>
+  <si>
+    <t>SWITCH ROCKER DPDT 15A 125V</t>
+  </si>
+  <si>
+    <t>PANEL MOUNT</t>
   </si>
 </sst>
 </file>
@@ -590,17 +590,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C911C1E-4B8A-41E6-9DEB-A7702C0270F1}">
-  <dimension ref="A1:E16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B74CCD21-E8D4-4A68-A154-31AE7F41C2DF}">
+  <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" customWidth="1"/>
-    <col min="2" max="2" width="38.140625" customWidth="1"/>
+    <col min="1" max="1" width="22.7109375" customWidth="1"/>
+    <col min="2" max="2" width="37.85546875" customWidth="1"/>
     <col min="3" max="5" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -660,13 +660,13 @@
         <v>13</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>58</v>
+        <v>14</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>57</v>
+        <v>16</v>
       </c>
       <c r="E4" s="3">
         <v>1</v>
@@ -674,16 +674,16 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>55</v>
+        <v>14</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>56</v>
       </c>
       <c r="E5" s="3">
         <v>1</v>
@@ -691,16 +691,16 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>17</v>
       </c>
       <c r="E6" s="3">
         <v>1</v>
@@ -708,16 +708,16 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C7" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>20</v>
       </c>
       <c r="E7" s="3">
         <v>1</v>
@@ -725,16 +725,16 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E8" s="3">
         <v>1</v>
@@ -742,16 +742,16 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C9" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>26</v>
       </c>
       <c r="E9" s="3">
         <v>1</v>
@@ -759,16 +759,16 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B10" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>50</v>
       </c>
       <c r="E10" s="3">
         <v>2</v>
@@ -776,13 +776,13 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>51</v>
@@ -793,16 +793,16 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E12" s="3">
         <v>2</v>
@@ -810,16 +810,16 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B13" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>41</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>40</v>
       </c>
       <c r="E13" s="3">
         <v>1</v>
@@ -827,16 +827,16 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="B14" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C14" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="D14" s="2" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="E14" s="3">
         <v>1</v>
@@ -844,16 +844,16 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="E15" s="3">
         <v>2</v>
@@ -861,18 +861,52 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="E16" s="3">
+      <c r="E16" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E17" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E18" s="2">
         <v>1</v>
       </c>
     </row>

</xml_diff>